<commit_message>
replacement and Update Project
</commit_message>
<xml_diff>
--- a/Documents/REsgraphical summary project charter.xlsx
+++ b/Documents/REsgraphical summary project charter.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelapinzonc/Desktop/UPT PRIN/Licenciatura/Primer ano/Primer Semestre/PROJETO AMIS/REPO Y FUENTES/Project-AMIS-MC-LP/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F763535F-F500-9646-92C1-E58A4F917F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BAE15F-88BB-4444-A79D-2EC8437AE9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2650258F-1F87-3D4E-9A71-00EA5126B128}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{2650258F-1F87-3D4E-9A71-00EA5126B128}"/>
   </bookViews>
   <sheets>
-    <sheet name="Diagrama Grannt" sheetId="2" r:id="rId1"/>
-    <sheet name="Project Charter" sheetId="1" r:id="rId2"/>
+    <sheet name="Project Charter" sheetId="2" r:id="rId1"/>
+    <sheet name="Driagrama de Gannt" sheetId="1" r:id="rId2"/>
+    <sheet name="Budget Baseline" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>Informacion del Proyecto</t>
   </si>
@@ -99,6 +100,244 @@
   </si>
   <si>
     <t>€ 40.000</t>
+  </si>
+  <si>
+    <t>CONCEPT</t>
+  </si>
+  <si>
+    <t>TOTAL BASELINE</t>
+  </si>
+  <si>
+    <t>TOTAL BUDGET</t>
+  </si>
+  <si>
+    <t>WBS</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>1.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2. </t>
+  </si>
+  <si>
+    <t>1.3.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>2.1.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>1.4.</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3.</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>Software Licenses</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Development team</t>
+    </r>
+  </si>
+  <si>
+    <t>Testing Staff</t>
+  </si>
+  <si>
+    <t>Project management</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Operations team</t>
+    </r>
+  </si>
+  <si>
+    <t>Project manager</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Hardware </t>
+    </r>
+  </si>
+  <si>
+    <t>Computer equipment</t>
+  </si>
+  <si>
+    <t>External consultancy</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>Specialized consultants</t>
+    </r>
+  </si>
+  <si>
+    <t>4.1.</t>
+  </si>
+  <si>
+    <t>5.1.</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>General expenses</t>
+  </si>
+  <si>
+    <t>Staff Training</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>6.1.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>Contingencies (10%)</t>
+  </si>
+  <si>
+    <t>TOTAL VALUE (EUR)</t>
+  </si>
+  <si>
+    <t>mo1</t>
+  </si>
+  <si>
+    <t>mo2</t>
+  </si>
+  <si>
+    <t>mo3</t>
+  </si>
+  <si>
+    <t>mo4</t>
+  </si>
+  <si>
+    <t>mo5</t>
+  </si>
+  <si>
+    <t>mo6</t>
+  </si>
+  <si>
+    <t>mo7</t>
+  </si>
+  <si>
+    <t>mo8</t>
+  </si>
+  <si>
+    <t>mo9</t>
+  </si>
+  <si>
+    <t>6.2.</t>
+  </si>
+  <si>
+    <t>6.3.</t>
+  </si>
+  <si>
+    <t>Supplies</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
   </si>
 </sst>
 </file>
@@ -106,9 +345,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,8 +373,74 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF767171"/>
+      <name val="Avenir Next Medium Italic"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF767171"/>
+      <name val="Avenir Next Medium Italic"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +459,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -314,76 +625,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,11 +1068,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B5A8E1-3856-5948-BEBC-C7B9B655D9B9}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="53.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="55.5" style="1" customWidth="1"/>
@@ -713,360 +1081,366 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:5" ht="22" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="21" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="20"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="20"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" ht="25" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="20" t="s">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" ht="23" customHeight="1">
+      <c r="A6" s="20"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="20"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="25" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="21" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="22" customHeight="1">
+      <c r="A9" s="20"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="20" t="s">
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="20"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" ht="25" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="20"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="20"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" ht="25" customHeight="1">
+      <c r="A14" s="2"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" ht="22" customHeight="1">
+      <c r="A15" s="20"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="22" customHeight="1">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="22" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="21"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33" spans="1:5" ht="22" customHeight="1">
+      <c r="A33" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="42" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="24">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="42" spans="1:5" ht="17" thickBot="1"/>
+    <row r="43" spans="1:5" ht="17" thickBot="1">
+      <c r="B43" s="6">
         <v>200</v>
       </c>
-      <c r="D43" s="26">
+      <c r="D43" s="8">
         <v>200000</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="25">
+    <row r="44" spans="1:5" ht="17" thickBot="1">
+      <c r="B44" s="7">
         <v>80</v>
       </c>
-      <c r="D44" s="26">
+      <c r="D44" s="8">
         <v>80000</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="25" t="s">
+    <row r="45" spans="1:5" ht="18" thickBot="1">
+      <c r="B45" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="8">
         <v>50000</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="25" t="s">
+    <row r="46" spans="1:5" ht="18" thickBot="1">
+      <c r="B46" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="26">
+      <c r="D46" s="8">
         <v>80000</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+    <row r="47" spans="1:5" ht="18" thickBot="1">
+      <c r="B47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="26">
+      <c r="D47" s="8">
         <v>70000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="25" t="s">
+    <row r="48" spans="1:5" ht="18" thickBot="1">
+      <c r="B48" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="8">
         <v>50000</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="25" t="s">
+    <row r="49" spans="2:4" ht="18" thickBot="1">
+      <c r="B49" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="26">
+      <c r="D49" s="8">
         <v>100000</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="25" t="s">
+    <row r="50" spans="2:4" ht="18" thickBot="1">
+      <c r="B50" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="26">
+      <c r="D50" s="8">
         <v>30000</v>
       </c>
     </row>
-    <row r="51" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="25" t="s">
+    <row r="51" spans="2:4" ht="18" thickBot="1">
+      <c r="B51" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="26">
+      <c r="D51" s="8">
         <v>40000</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D52" s="26">
+    <row r="52" spans="2:4">
+      <c r="D52" s="8">
         <f>+D43+D44+D45+D46+D47+D48+D49+D50+D51</f>
         <v>700000</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D53" s="26">
+    <row r="53" spans="2:4">
+      <c r="D53" s="8">
         <f>+D52*10%</f>
         <v>70000</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D54" s="26">
+    <row r="54" spans="2:4">
+      <c r="D54" s="8">
         <f>D52+D53</f>
         <v>770000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D22:E22"/>
@@ -1083,12 +1457,6 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1098,10 +1466,576 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBC367F-829E-724E-AA69-6DD07D418ACA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{775AEB21-D5D9-914A-AF9D-7F5E0AA4F375}">
+  <dimension ref="A2:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="12" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="19" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19" customHeight="1">
+      <c r="A3" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="32">
+        <f>C4+C5+C6+C7</f>
+        <v>141500</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" ht="19" customHeight="1">
+      <c r="A4" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="27">
+        <v>22500</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" ht="19" customHeight="1">
+      <c r="A5" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="27">
+        <v>39000</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" ht="19" customHeight="1">
+      <c r="A6" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="27">
+        <v>40000</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="1:12" ht="19" customHeight="1">
+      <c r="A7" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="27">
+        <v>40000</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="1:12" ht="19" customHeight="1">
+      <c r="A8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="32">
+        <f>C9+C10+C11</f>
+        <v>20000</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" ht="19" customHeight="1">
+      <c r="A9" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="27">
+        <v>20000</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+    </row>
+    <row r="10" spans="1:12" ht="19" customHeight="1">
+      <c r="A10" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" ht="19" customHeight="1">
+      <c r="A11" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+    </row>
+    <row r="12" spans="1:12" ht="19" customHeight="1">
+      <c r="A12" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="32">
+        <f>C13+C14+C15</f>
+        <v>50000</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+    </row>
+    <row r="13" spans="1:12" ht="19" customHeight="1">
+      <c r="A13" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="27">
+        <v>50000</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+    </row>
+    <row r="14" spans="1:12" ht="19" customHeight="1">
+      <c r="A14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="1:12" ht="19" customHeight="1">
+      <c r="A15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+    </row>
+    <row r="16" spans="1:12" ht="19" customHeight="1">
+      <c r="A16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="32">
+        <f>C17</f>
+        <v>100000</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:12" ht="19" customHeight="1">
+      <c r="A17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="27">
+        <v>100000</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="1:12" ht="19" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="32">
+        <f>C19</f>
+        <v>30000</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+    </row>
+    <row r="19" spans="1:12" ht="19" customHeight="1">
+      <c r="A19" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="27">
+        <v>30000</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+    </row>
+    <row r="20" spans="1:12" ht="19" customHeight="1">
+      <c r="A20" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="35">
+        <f>C21+C22+C23</f>
+        <v>40000</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+    </row>
+    <row r="21" spans="1:12" ht="19" customHeight="1">
+      <c r="A21" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="27">
+        <v>40000</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+    </row>
+    <row r="22" spans="1:12" ht="18">
+      <c r="A22" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+    </row>
+    <row r="23" spans="1:12" ht="18">
+      <c r="A23" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+    </row>
+    <row r="24" spans="1:12" ht="19" customHeight="1">
+      <c r="A24" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="27">
+        <v>700000</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+    </row>
+    <row r="25" spans="1:12" ht="19" customHeight="1">
+      <c r="A25" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+    </row>
+    <row r="26" spans="1:12" ht="19" customHeight="1">
+      <c r="A26" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="27">
+        <v>70000</v>
+      </c>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+    </row>
+    <row r="27" spans="1:12" ht="19" customHeight="1">
+      <c r="A27" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="27">
+        <v>770000</v>
+      </c>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35">
+        <f>C33+C34</f>
+        <v>61500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A24:B24"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>